<commit_message>
remove rogue link to old gh classrom
</commit_message>
<xml_diff>
--- a/C4RM_Class_04.xlsx
+++ b/C4RM_Class_04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidromoff/Downloads/AA/GoodStuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CarbonX1\Documents\GitHub\C4RM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065C5984-8401-2443-819B-4B1C9F1E35AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4885E5BA-C76D-48D2-B1C9-58BA652AD537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C1F6CC11-1296-3549-A35C-9D74F73648F5}"/>
+    <workbookView xWindow="6975" yWindow="4125" windowWidth="22080" windowHeight="15255" firstSheet="10" activeTab="16" xr2:uid="{C1F6CC11-1296-3549-A35C-9D74F73648F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Today" sheetId="29" r:id="rId1"/>
@@ -893,7 +893,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1192,7 +1192,6 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{277ED423-15D8-FE49-8E22-F8A124002D26}"/>
@@ -1356,7 +1355,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F72CF731-9F75-444E-825B-785A22B5D870}"/>
@@ -4364,71 +4363,16 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Terminology"/>
-      <sheetName val="NormalEquations"/>
+      <sheetName val="RSquareAdj"/>
+      <sheetName val="QualityOfFit"/>
       <sheetName val="ExcelOutput"/>
-      <sheetName val="DegreesOfFreedom"/>
-      <sheetName val="QualityOfFit"/>
-      <sheetName val="RSquareAdj"/>
-      <sheetName val="FTest"/>
-      <sheetName val="OrdinaryLeastSquares"/>
       <sheetName val="MaximumLikelihood"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="C1">
-            <v>-2</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="C1">
-            <v>-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="6">
-          <cell r="C6">
-            <v>0.8</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>0.19999999999999996</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>1.0555555555555556</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0.21111111111111108</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7">
-        <row r="3">
-          <cell r="E3">
-            <v>20</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="3">
-          <cell r="C3">
-            <v>0.2888819048927293</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4438,66 +4382,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Today"/>
-      <sheetName val="SetUp"/>
-      <sheetName val="Macro"/>
-      <sheetName val="Looping"/>
-      <sheetName val="Conditioning"/>
-      <sheetName val="Functions"/>
-      <sheetName val="Computer"/>
-      <sheetName val="DataTypes"/>
-      <sheetName val="Mechanics"/>
-      <sheetName val="Arrays"/>
-      <sheetName val="qOffice1_Filter"/>
-      <sheetName val="qOffice_Pivot"/>
-      <sheetName val="Prework4NextClass"/>
-      <sheetName val="InClassProjects"/>
       <sheetName val="qFunctions"/>
-      <sheetName val="qArrays1"/>
-      <sheetName val="qDataTypes"/>
-      <sheetName val="qConditioning"/>
-      <sheetName val="BLANK"/>
-      <sheetName val="DataTypes_ASCII"/>
-      <sheetName val="NextTime"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14">
-        <row r="6">
-          <cell r="C6">
-            <v>2000000</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>0.03</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>0.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4868,47 +4756,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Class3"/>
-      <sheetName val="Objectives3"/>
       <sheetName val="FX_Intro"/>
-      <sheetName val="CoveredInterestParity"/>
-      <sheetName val="FXQuotation"/>
-      <sheetName val="QuizBank"/>
-      <sheetName val="Homework"/>
-      <sheetName val="O_Material"/>
-      <sheetName val="O_Discussion"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="65">
-          <cell r="C65">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>0.08</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>0.04</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>2.0769230769230771</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4933,1486 +4784,16 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Today"/>
-      <sheetName val="Normal"/>
-      <sheetName val="Normal_Excel"/>
-      <sheetName val="Intuition1"/>
-      <sheetName val="Intuition2"/>
-      <sheetName val="Intuition3"/>
-      <sheetName val="Methods1"/>
-      <sheetName val="Methods2"/>
-      <sheetName val="Calcs_Mean1"/>
       <sheetName val="Calcs_Mean2"/>
       <sheetName val="Calcs_MeanDiff"/>
       <sheetName val="Calcs_VarianceDiff"/>
-      <sheetName val="NextClass"/>
-      <sheetName val="PreWork4NextClass"/>
-      <sheetName val="Drills"/>
-      <sheetName val="ClassWork"/>
-      <sheetName val="1_Stats"/>
-      <sheetName val="2_MeanSigmaKnown"/>
-      <sheetName val="3_MeanSigmaUnknown"/>
-      <sheetName val="4_TwoMeans"/>
-      <sheetName val="5_BacktestMean"/>
-      <sheetName val="FinalExamReview"/>
-      <sheetName val="ClassPolicy"/>
-      <sheetName val="Programming"/>
-      <sheetName val="ProgrammingAnswer_R"/>
-      <sheetName val="1_MeanSigmaKnown"/>
-      <sheetName val="2_MeanSigmaUnknown"/>
-      <sheetName val="3_TwoMeans"/>
-      <sheetName val="4_BacktestMean"/>
-      <sheetName val="4_Backtest"/>
+      <sheetName val="Calcs_Mean1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8">
-        <row r="21">
-          <cell r="O21">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="O29">
-            <v>-9.3105936164507597</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="10">
-          <cell r="C10">
-            <v>71.222704059275372</v>
-          </cell>
-          <cell r="K10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>69.592590560721447</v>
-          </cell>
-          <cell r="K11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>69.171701116206393</v>
-          </cell>
-          <cell r="K12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>69.886811841441983</v>
-          </cell>
-          <cell r="K13">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>72.095059632317273</v>
-          </cell>
-          <cell r="K14">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>68.71442093827325</v>
-          </cell>
-          <cell r="K15">
-            <v>6</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>67.511488956444168</v>
-          </cell>
-          <cell r="K16">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>67.80390447486333</v>
-          </cell>
-          <cell r="K17">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>69.245440893422384</v>
-          </cell>
-          <cell r="K18">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>67.486969775791792</v>
-          </cell>
-          <cell r="K19">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>65.726288352833677</v>
-          </cell>
-          <cell r="K20">
-            <v>16</v>
-          </cell>
-          <cell r="O20">
-            <v>68.19602794463934</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>66.018996336968542</v>
-          </cell>
-          <cell r="K21">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>73.909318116793344</v>
-          </cell>
-          <cell r="K22">
-            <v>11</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>69.811447220932024</v>
-          </cell>
-          <cell r="K23">
-            <v>6</v>
-          </cell>
-          <cell r="O23">
-            <v>70</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>68.704207627980921</v>
-          </cell>
-          <cell r="K24">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>71.577904534604286</v>
-          </cell>
-          <cell r="K25">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>68.987160667245945</v>
-          </cell>
-          <cell r="K26">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>68.139407647556311</v>
-          </cell>
-          <cell r="K27">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>68.263303535487012</v>
-          </cell>
-          <cell r="K28">
-            <v>1</v>
-          </cell>
-          <cell r="O28">
-            <v>0.18827338580548053</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>69.298964805666813</v>
-          </cell>
-          <cell r="K29">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>69.539151316452831</v>
-          </cell>
-          <cell r="K30">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>69.88118428502932</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>67.756769947600134</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>66.376308331312686</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>68.517908635291761</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>67.176335799544432</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>70.415547610037279</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>66.641133397163529</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>65.412760760643977</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>66.032863657633825</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>66.062225895065012</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>68.982952489547841</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>66.974239665427405</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>68.853158106914321</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>70.432995512140366</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>69.579299462652926</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>69.64297816342922</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>66.128478998692785</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>67.088795754199452</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>68.5509594973812</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>68.857253603534062</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>68.908110446552669</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>66.659441774501317</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>70.888747042962166</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>66.662217014214619</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55">
-            <v>69.443545321587251</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56">
-            <v>65.317310019833698</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>70.070652963575014</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>68.066303419346966</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>69.705626880851014</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>70.166874042397652</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>71.117242640941711</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>68.437067932602758</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>68.539947100113963</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>64.188656827572402</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>69.955064984293955</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>66.746719582985932</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>67.590767916782511</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>67.0026153944589</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>68.89727318447936</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>66.240799836049845</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>67.622123312215663</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>68.011594143719293</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>65.079552318153816</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>68.191617814212336</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>65.453393107574044</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>64.701590959544774</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>65.032657870426192</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>66.866136438790662</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79">
-            <v>69.058517012006291</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="C80">
-            <v>66.402213707115507</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="C81">
-            <v>69.997040942469823</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="C82">
-            <v>66.216952837834071</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="C83">
-            <v>67.730371627898421</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="C84">
-            <v>69.666251154459914</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="C85">
-            <v>68.990161299691067</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="C86">
-            <v>70.885113562671862</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="C87">
-            <v>68.837941179053828</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="C88">
-            <v>68.161072368310286</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="C89">
-            <v>65.674508989197008</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="C90">
-            <v>69.051450571206871</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="C91">
-            <v>68.288231788470611</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="C92">
-            <v>68.896238533554296</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="C93">
-            <v>66.266741537612248</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="C94">
-            <v>70.588099195452173</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="C95">
-            <v>70.215376294783667</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="C96">
-            <v>65.616312664691804</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="C97">
-            <v>70.611090333534975</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="C98">
-            <v>70.218142748306263</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="C99">
-            <v>64.316476310303443</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="C100">
-            <v>65.948657745899951</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="C101">
-            <v>68.000040590588611</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="C102">
-            <v>69.482252970993812</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="C103">
-            <v>69.735017836342777</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="C104">
-            <v>67.081667923554122</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="C105">
-            <v>68.546256125289673</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="C106">
-            <v>67.412833594648333</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="C107">
-            <v>67.088240140800323</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="C108">
-            <v>68.094912132938745</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="C109">
-            <v>64.889568468993559</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10">
-        <row r="10">
-          <cell r="C10">
-            <v>69.636713419029206</v>
-          </cell>
-          <cell r="D10">
-            <v>71.955870295235684</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>65.448684903785278</v>
-          </cell>
-          <cell r="D11">
-            <v>72.088168016484488</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>67.422541587634299</v>
-          </cell>
-          <cell r="D12">
-            <v>68.067804641860945</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>66.906068567438254</v>
-          </cell>
-          <cell r="D13">
-            <v>68.191420112242369</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>68.08116991283147</v>
-          </cell>
-          <cell r="D14">
-            <v>71.673141413412054</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>67.165125888370923</v>
-          </cell>
-          <cell r="D15">
-            <v>72.509843575402215</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>67.997528895991138</v>
-          </cell>
-          <cell r="D16">
-            <v>68.712852920465977</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>70.973398062336472</v>
-          </cell>
-          <cell r="D17">
-            <v>68.738266259630151</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>68.848521927352749</v>
-          </cell>
-          <cell r="D18">
-            <v>68.924825931662909</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>67.107323107390741</v>
-          </cell>
-          <cell r="D19">
-            <v>70.760681367788152</v>
-          </cell>
-          <cell r="R19">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>68.28516501091508</v>
-          </cell>
-          <cell r="D20">
-            <v>70.844641725898441</v>
-          </cell>
-          <cell r="R20">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>70.28446793343609</v>
-          </cell>
-          <cell r="D21">
-            <v>68.291389524484401</v>
-          </cell>
-          <cell r="R21">
-            <v>68.212317190546059</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>67.254486584130376</v>
-          </cell>
-          <cell r="D22">
-            <v>71.643187497462023</v>
-          </cell>
-          <cell r="R22">
-            <v>70.032144729678777</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>67.190102095930484</v>
-          </cell>
-          <cell r="D23">
-            <v>68.996403457563034</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>67.604041046576739</v>
-          </cell>
-          <cell r="D24">
-            <v>71.776296026494322</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>68.404322937460506</v>
-          </cell>
-          <cell r="D25">
-            <v>68.444236626911902</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>68.368738773103871</v>
-          </cell>
-          <cell r="D26">
-            <v>70.424356413421947</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>69.38439199690707</v>
-          </cell>
-          <cell r="D27">
-            <v>70.427871668169843</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>65.861911573963383</v>
-          </cell>
-          <cell r="D28">
-            <v>68.602071185152468</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>67.135236061381008</v>
-          </cell>
-          <cell r="D29">
-            <v>68.293519831591041</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>69.385537582639202</v>
-          </cell>
-          <cell r="D30">
-            <v>69.495629008158218</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>70.458100367462819</v>
-          </cell>
-          <cell r="D31">
-            <v>71.968776397777489</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>66.527056179799743</v>
-          </cell>
-          <cell r="D32">
-            <v>67.635410735970382</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>66.384631972484456</v>
-          </cell>
-          <cell r="D33">
-            <v>68.262198258011495</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>72.185439467946992</v>
-          </cell>
-          <cell r="D34">
-            <v>69.490289461608256</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>68.26063364495937</v>
-          </cell>
-          <cell r="D35">
-            <v>72.044669722299076</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>67.759109276605287</v>
-          </cell>
-          <cell r="D36">
-            <v>71.770089503712214</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>70.530729781092248</v>
-          </cell>
-          <cell r="D37">
-            <v>67.441963663222737</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>66.773496982972446</v>
-          </cell>
-          <cell r="D38">
-            <v>68.283639247621778</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>66.089240229389233</v>
-          </cell>
-          <cell r="D39">
-            <v>69.295789280070849</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>73.553545521118735</v>
-          </cell>
-          <cell r="D40">
-            <v>69.787189658683687</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>71.319151506755787</v>
-          </cell>
-          <cell r="D41">
-            <v>68.845875044689691</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>68.12935685087777</v>
-          </cell>
-          <cell r="D42">
-            <v>69.315641965706064</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>67.476128212092732</v>
-          </cell>
-          <cell r="D43">
-            <v>68.147137729220901</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>67.878779722301701</v>
-          </cell>
-          <cell r="D44">
-            <v>68.967370481077737</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>69.292375263267942</v>
-          </cell>
-          <cell r="D45">
-            <v>69.701617586439895</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>67.021659175779263</v>
-          </cell>
-          <cell r="D46">
-            <v>70.004945355647536</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>69.249321959130455</v>
-          </cell>
-          <cell r="D47">
-            <v>69.510071151332255</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>68.272269617442674</v>
-          </cell>
-          <cell r="D48">
-            <v>70.635061719408796</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>66.609403882413829</v>
-          </cell>
-          <cell r="D49">
-            <v>68.444100814694906</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>65.779961877071898</v>
-          </cell>
-          <cell r="D50">
-            <v>70.883354087886659</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>71.900872564649205</v>
-          </cell>
-          <cell r="D51">
-            <v>68.995890507181187</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>66.614779486248949</v>
-          </cell>
-          <cell r="D52">
-            <v>70.551004826600561</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>67.201210663945673</v>
-          </cell>
-          <cell r="D53">
-            <v>71.701774142827759</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>67.621528957655684</v>
-          </cell>
-          <cell r="D54">
-            <v>72.402627736228141</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55">
-            <v>64.495444697763503</v>
-          </cell>
-          <cell r="D55">
-            <v>70.907617613041822</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56">
-            <v>69.362703640776047</v>
-          </cell>
-          <cell r="D56">
-            <v>69.796962402834595</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>70.689475849512519</v>
-          </cell>
-          <cell r="D57">
-            <v>72.392993625081857</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>64.221951420923645</v>
-          </cell>
-          <cell r="D58">
-            <v>70.296488743990025</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>66.838179172843553</v>
-          </cell>
-          <cell r="D59">
-            <v>69.33761274865428</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>66.978119045660648</v>
-          </cell>
-          <cell r="D60">
-            <v>72.221643586092199</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>67.064577694142983</v>
-          </cell>
-          <cell r="D61">
-            <v>67.578929089382342</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>66.878397270685056</v>
-          </cell>
-          <cell r="D62">
-            <v>68.004754782366575</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>67.749220652855882</v>
-          </cell>
-          <cell r="D63">
-            <v>69.934160844975537</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>67.691621108876731</v>
-          </cell>
-          <cell r="D64">
-            <v>71.124837438515442</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>66.594574979176443</v>
-          </cell>
-          <cell r="D65">
-            <v>71.219304577658534</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>65.175871772551218</v>
-          </cell>
-          <cell r="D66">
-            <v>65.995936457135045</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>70.039953524939918</v>
-          </cell>
-          <cell r="D67">
-            <v>68.435621625880046</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>67.992315376848552</v>
-          </cell>
-          <cell r="D68">
-            <v>71.095512053969841</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>69.241731918144723</v>
-          </cell>
-          <cell r="D69">
-            <v>69.766464555920692</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>65.000015025044661</v>
-          </cell>
-          <cell r="D70">
-            <v>68.270796497839939</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>72.072968621434455</v>
-          </cell>
-          <cell r="D71">
-            <v>68.99296430869083</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>73.059783706605074</v>
-          </cell>
-          <cell r="D72">
-            <v>70.063742579725641</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>66.997443852275282</v>
-          </cell>
-          <cell r="D73">
-            <v>70.782170104044525</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>70.265182596670215</v>
-          </cell>
-          <cell r="D74">
-            <v>70.997412350510373</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>66.501268694840235</v>
-          </cell>
-          <cell r="D75">
-            <v>70.667856526165195</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>65.522279818116175</v>
-          </cell>
-          <cell r="D76">
-            <v>70.28033106535095</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>66.327280468287128</v>
-          </cell>
-          <cell r="D77">
-            <v>69.774472880884005</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>68.975861583296179</v>
-          </cell>
-          <cell r="D78">
-            <v>69.456784067467396</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79">
-            <v>74.128186536020976</v>
-          </cell>
-          <cell r="D79">
-            <v>71.660606432734241</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="C80">
-            <v>68.228424067072979</v>
-          </cell>
-          <cell r="D80">
-            <v>71.33232298759161</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="C81">
-            <v>66.761427272563978</v>
-          </cell>
-          <cell r="D81">
-            <v>72.616244624420375</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="C82">
-            <v>68.608070928545743</v>
-          </cell>
-          <cell r="D82">
-            <v>69.568953494564212</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="C83">
-            <v>68.767904037551361</v>
-          </cell>
-          <cell r="D83">
-            <v>71.12814319475001</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="C84">
-            <v>67.947195347852755</v>
-          </cell>
-          <cell r="D84">
-            <v>69.982158127359</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="C85">
-            <v>66.36480344870391</v>
-          </cell>
-          <cell r="D85">
-            <v>69.707084136669053</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="C86">
-            <v>67.237578058670735</v>
-          </cell>
-          <cell r="D86">
-            <v>70.763652121273324</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="C87">
-            <v>70.900868413699214</v>
-          </cell>
-          <cell r="D87">
-            <v>70.378242884626445</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="C88">
-            <v>67.908767189083534</v>
-          </cell>
-          <cell r="D88">
-            <v>72.562404625090224</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="C89">
-            <v>69.185199185658405</v>
-          </cell>
-          <cell r="D89">
-            <v>68.329197512940922</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="C90">
-            <v>67.95871707918522</v>
-          </cell>
-          <cell r="D90">
-            <v>68.013121854068444</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="C91">
-            <v>66.979916275544383</v>
-          </cell>
-          <cell r="D91">
-            <v>68.588413750088492</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="C92">
-            <v>68.069804949520844</v>
-          </cell>
-          <cell r="D92">
-            <v>73.631495535813116</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="C93">
-            <v>65.773879854787211</v>
-          </cell>
-          <cell r="D93">
-            <v>67.549452167535847</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="C94">
-            <v>65.631274238364725</v>
-          </cell>
-          <cell r="D94">
-            <v>71.710537227422662</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="C95">
-            <v>69.35704956444917</v>
-          </cell>
-          <cell r="D95">
-            <v>72.326182817926195</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="C96">
-            <v>66.764066427763595</v>
-          </cell>
-          <cell r="D96">
-            <v>68.738508807128511</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="C97">
-            <v>70.040534832916009</v>
-          </cell>
-          <cell r="D97">
-            <v>70.12039207215399</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="C98">
-            <v>68.062720112100067</v>
-          </cell>
-          <cell r="D98">
-            <v>71.989618818211454</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="C99">
-            <v>67.36112687270932</v>
-          </cell>
-          <cell r="D99">
-            <v>70.699388147479269</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="C100">
-            <v>70.532949243170847</v>
-          </cell>
-          <cell r="D100">
-            <v>71.649402835701764</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="C101">
-            <v>68.922565375150484</v>
-          </cell>
-          <cell r="D101">
-            <v>67.025477203643277</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="C102">
-            <v>70.408226065643603</v>
-          </cell>
-          <cell r="D102">
-            <v>69.291995020633863</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="C103">
-            <v>67.499864121352203</v>
-          </cell>
-          <cell r="D103">
-            <v>70.757771050164024</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="C104">
-            <v>72.340262111685689</v>
-          </cell>
-          <cell r="D104">
-            <v>72.109391143380023</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="C105">
-            <v>68.086419180312788</v>
-          </cell>
-          <cell r="D105">
-            <v>68.008632746184205</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="C106">
-            <v>65.517824954735175</v>
-          </cell>
-          <cell r="D106">
-            <v>70.496797876759103</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="C107">
-            <v>69.921821712167684</v>
-          </cell>
-          <cell r="D107">
-            <v>67.157069767832283</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="C108">
-            <v>71.291395354164806</v>
-          </cell>
-          <cell r="D108">
-            <v>73.885543024984855</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="C109">
-            <v>67.302392719119482</v>
-          </cell>
-          <cell r="D109">
-            <v>71.091933855155474</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="13">
-          <cell r="E13">
-            <v>4.05591218745404</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>16.040841688285191</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>0.25284908773933717</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>2.3476972799816505E-11</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6437,201 +4818,14 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Prep"/>
       <sheetName val="Bond"/>
+      <sheetName val="Dur2"/>
       <sheetName val="InstallmentLoan"/>
-      <sheetName val="Duration"/>
-      <sheetName val="Dur2"/>
-      <sheetName val="Dur3"/>
-      <sheetName val="Curve0"/>
-      <sheetName val="Remember"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="C4">
-            <v>2000000</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>2.5000000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="E21">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>35000</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>2035000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="3">
-          <cell r="F3">
-            <v>10.837769560171987</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="12">
-          <cell r="G12">
-            <v>0.98760555034319286</v>
-          </cell>
-          <cell r="I12">
-            <v>2126382.9183726022</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="G13">
-            <v>0.97536472306868083</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="G14">
-            <v>0.96327561411158036</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="G15">
-            <v>0.95133634300684455</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="G16">
-            <v>0.93954505259675514</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="G17">
-            <v>0.92789990874204242</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="G18">
-            <v>0.9163991000365832</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="G19">
-            <v>0.90504083752563647</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="G20">
-            <v>0.89382335442757033</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="G21">
-            <v>0.88274490585903931</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="G22">
-            <v>0.87180376856356656</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="G23">
-            <v>0.86099824064349073</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="G24">
-            <v>0.85032664129523539</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="G25">
-            <v>0.83978731054785982</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
-        <row r="26">
-          <cell r="E26">
-            <v>1200.2040073638184</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6656,89 +4850,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Class10"/>
-      <sheetName val="LearningObjectives"/>
-      <sheetName val="Concepts1"/>
-      <sheetName val="RiskDrivers"/>
-      <sheetName val="SourcesOfLiquidity"/>
-      <sheetName val="Concepts2"/>
-      <sheetName val="Liquidity"/>
-      <sheetName val="Scenario"/>
-      <sheetName val="Ratios"/>
-      <sheetName val="Matz_Ch2"/>
-      <sheetName val="Matz_Ch4"/>
-      <sheetName val="Matz_Ch7"/>
-      <sheetName val="StressTesting"/>
-      <sheetName val="LCR"/>
-      <sheetName val="LCR_Calc"/>
-      <sheetName val="NSFR"/>
       <sheetName val="ASF"/>
-      <sheetName val="RSF"/>
-      <sheetName val="IMix1"/>
-      <sheetName val="IMix1Calc"/>
-      <sheetName val="IMix2"/>
-      <sheetName val="IMix2Calc"/>
-      <sheetName val="O_Discussion"/>
-      <sheetName val="Bonus"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16" refreshError="1">
-        <row r="31">
-          <cell r="C31">
-            <v>1</v>
-          </cell>
-          <cell r="D31" t="str">
-            <v>Amount</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>2</v>
-          </cell>
-          <cell r="D32" t="str">
-            <v>of</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>3</v>
-          </cell>
-          <cell r="D33" t="str">
-            <v>Stable</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>4</v>
-          </cell>
-          <cell r="D34" t="str">
-            <v>Funding</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6749,43 +4864,9 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="2_PMT"/>
-      <sheetName val="Today"/>
-      <sheetName val="GeometricSeries"/>
-      <sheetName val="NextClass"/>
-      <sheetName val="PreWork4NextClass"/>
-      <sheetName val="ClassWork"/>
-      <sheetName val="1_GeoSeries"/>
-      <sheetName val="3_IncreaseAnnuity"/>
-      <sheetName val="4_Dice"/>
-      <sheetName val="5_ConditionalProb"/>
-      <sheetName val="5_ConditionalProb (2)"/>
-      <sheetName val="FinalExamReview"/>
-      <sheetName val="ClassPolicy"/>
-      <sheetName val="Programming"/>
-      <sheetName val="ProgrammingAnswer_R"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="13">
-          <cell r="C13">
-            <v>0.90909090909090906</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6795,590 +4876,12 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Today"/>
-      <sheetName val="TMat1"/>
-      <sheetName val="TMat2"/>
-      <sheetName val="TMat3"/>
+      <sheetName val="NextClass1_MeanVar"/>
       <sheetName val="Binomial"/>
-      <sheetName val="Normal"/>
-      <sheetName val="NextClass1_MeanVar"/>
-      <sheetName val="NextClass2_CovCorr"/>
-      <sheetName val="NextClass3_SkewKurt"/>
-      <sheetName val="NextClass4_Videos"/>
-      <sheetName val="PreWork4NextClass"/>
-      <sheetName val="ClassWork"/>
-      <sheetName val="1_Vote"/>
-      <sheetName val="2_TMatrix"/>
-      <sheetName val="3_TMatrix2"/>
-      <sheetName val="4_ConditionalProbability"/>
-      <sheetName val="5_DenomSwitch"/>
-      <sheetName val="6_Normal"/>
-      <sheetName val="7_Backtest"/>
-      <sheetName val="8_LifeAnnuity"/>
-      <sheetName val="FinalExamReview"/>
-      <sheetName val="ClassPolicy"/>
-      <sheetName val="Programming"/>
-      <sheetName val="Programming_Data"/>
-      <sheetName val="Programming_Answer_P"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
-        <row r="12">
-          <cell r="C12">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>0.02</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6">
-        <row r="24">
-          <cell r="E24">
-            <v>-2.0344842309874376</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>2.6710696453581235</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>4.7055538763455615</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>0.47283563207088219</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>0.45767178102260736</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>0.42492062610286929</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>0.59889153009821006</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>-0.53177593704778414</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>-1.0923730126346645</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>-1.5032931355800621</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>1.5847145107069514</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>-1.0653967582348218</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>-0.41124559773468478</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>-3.1141255841770681E-2</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>1.2468143389598696</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>0.13044182619797937</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>0.59193078372161201</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>0.82333603760006313</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>0.65275066245239</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>-1.3299123879368187</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>1.8144389682637543</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>0.18357809747018158</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>1.3548288082437756</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>0.96000378303928868</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>-0.75251590001080337</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>-0.54280595514466867</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>1.4450781934897143</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>-1.3103661952828956</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55">
-            <v>0.86453510799169753</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56">
-            <v>0.54063492010443293</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>-1.1926173327716567</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>-2.0344842309874376</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>1.7299667033107016</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>1.5877550893721093</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>0.65950770253534019</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>0.97540989122619604</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>0.36092288473141043</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>1.8562365796243729</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>-0.20913258218132988</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>-0.43135032447355126</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>-0.50537849528565904</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>1.2005463935897949</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>-0.95292427154916037</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>-1.489300177748593</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>1.3569249544412405</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>-3.4339261951630076E-2</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>0.47242793486658613</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>-0.20616730719777968</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>-0.1241253327308736</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>-0.15797703340739311</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>0.7834064814089936</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>-0.31403473645401986</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79">
-            <v>-1.0892091579210856</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="C80">
-            <v>-0.14229621061692244</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="C81">
-            <v>-0.95498011758643009</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="C82">
-            <v>2.4325997984353718</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="C83">
-            <v>-0.24005877903367401</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="C84">
-            <v>-0.54140727804528221</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="C85">
-            <v>0.71219161995211278</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="C86">
-            <v>0.48682362643606775</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="C87">
-            <v>0.41460686137681257</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="C88">
-            <v>1.002966196417018</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="C89">
-            <v>0.54243255375052368</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="C90">
-            <v>-1.8689342043077717</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="C91">
-            <v>-0.1275510652267782</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="C92">
-            <v>0.36656834921990267</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="C93">
-            <v>0.1959142079947935</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="C94">
-            <v>0.1633818377141269</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="C95">
-            <v>2.6710696453581235</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="C96">
-            <v>-0.42429971649028647</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="C97">
-            <v>-0.61637830092325185</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="C98">
-            <v>-1.2467608733272906</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="C99">
-            <v>-1.2420790016593952</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="C100">
-            <v>0.61925278950750406</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="C101">
-            <v>0.20992154625570031</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="C102">
-            <v>0.43154151978882149</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="C103">
-            <v>-0.61942148444040201</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="C104">
-            <v>0.31298184561513664</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="C105">
-            <v>-1.3293756011157096</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="C106">
-            <v>-0.71328480340091105</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="C107">
-            <v>1.3924790675406515</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="C108">
-            <v>1.1826914188463862</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="C109">
-            <v>1.4342383981022007</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="C110">
-            <v>0.78543422003077046</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="C111">
-            <v>-1.0870596324040505</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="C112">
-            <v>0.63325128160473498</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="C113">
-            <v>0.77787386482362986</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="C114">
-            <v>0.24837890304058732</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="C115">
-            <v>0.80752026146839906</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="C116">
-            <v>0.74478903054676848</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="C117">
-            <v>-1.1491720845402209</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="C118">
-            <v>0.42896914696081034</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="C119">
-            <v>-0.597892993359188</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="C120">
-            <v>0.88781240410706486</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="C121">
-            <v>1.4220282396798032</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="C122">
-            <v>1.5429318688961562</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="C123">
-            <v>0.34104768407371333</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="C124">
-            <v>0.99699934548788016</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="C125">
-            <v>-1.509506598426565</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="C126">
-            <v>-1.7004043615721947</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="C127">
-            <v>0.36438233854416907</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="C128">
-            <v>-0.68071196946934187</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="C129">
-            <v>-1.4717164307075286</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7388,28 +4891,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="3_Probability&amp;ThePublic"/>
       <sheetName val="InvestmentReturns"/>
-      <sheetName val="AVPlot"/>
-      <sheetName val="MaximumLikelihood"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="12">
-          <cell r="B12">
-            <v>10000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="3">
-          <cell r="B3">
-            <v>2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8220,42 +5705,12 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Intro"/>
-      <sheetName val="Intro1"/>
-      <sheetName val="Day1"/>
-      <sheetName val="Day2"/>
-      <sheetName val="Themes"/>
       <sheetName val="Excel"/>
-      <sheetName val="C0"/>
-      <sheetName val="C1"/>
       <sheetName val="VaR0"/>
-      <sheetName val="VaR1"/>
-      <sheetName val="Class6"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="10">
-          <cell r="C10">
-            <v>0.30509841009160843</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9">
-        <row r="17">
-          <cell r="H17">
-            <v>-0.1166666666666667</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8280,195 +5735,10 @@
     <sheetNames>
       <sheetName val="OptionsHW"/>
       <sheetName val="fxHW"/>
-      <sheetName val="VaR_HW_Q1"/>
-      <sheetName val="VaR_HW_Q2"/>
-      <sheetName val="VaR_HW_2.4"/>
-      <sheetName val="VaR_HW_1"/>
-      <sheetName val="VaR_HW_2"/>
-      <sheetName val="HW6"/>
-      <sheetName val="Date0"/>
-      <sheetName val="Date1"/>
-      <sheetName val="Date2"/>
-      <sheetName val="Date0Check1"/>
-      <sheetName val="Date0Check2"/>
-      <sheetName val="4.2"/>
-      <sheetName val="4.3"/>
-      <sheetName val="4.4"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2">
-            <v>67</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>0.38595880367242197</v>
-          </cell>
-          <cell r="D12">
-            <v>0.58659004994372632</v>
-          </cell>
-          <cell r="E12">
-            <v>0.37550388277557334</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>0.3121138317415072</v>
-          </cell>
-          <cell r="D13">
-            <v>0.5111143422154043</v>
-          </cell>
-          <cell r="E13">
-            <v>0.18107379394568301</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>0.61404119632757803</v>
-          </cell>
-          <cell r="D14">
-            <v>0.41340995005627368</v>
-          </cell>
-          <cell r="E14">
-            <v>0.62449611722442666</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>0.6878861682584928</v>
-          </cell>
-          <cell r="D15">
-            <v>0.48888565778459575</v>
-          </cell>
-          <cell r="E15">
-            <v>0.81892620605431699</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>65.837699789559906</v>
-          </cell>
-          <cell r="D17">
-            <v>775</v>
-          </cell>
-          <cell r="E17">
-            <v>237</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>71.176742801849741</v>
-          </cell>
-          <cell r="D18">
-            <v>756.96607190143357</v>
-          </cell>
-          <cell r="E18">
-            <v>341.35846920991639</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>3.1953939205575459</v>
-          </cell>
-          <cell r="D20">
-            <v>67.711072787108264</v>
-          </cell>
-          <cell r="E20">
-            <v>27.183347102480703</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>3000000</v>
-          </cell>
-          <cell r="D25">
-            <v>1000000</v>
-          </cell>
-          <cell r="E25">
-            <v>5000000</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>44776.119402985074</v>
-          </cell>
-          <cell r="D26">
-            <v>1290.3225806451612</v>
-          </cell>
-          <cell r="E26">
-            <v>21097.04641350211</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="F3">
-            <v>1.385</v>
-          </cell>
-          <cell r="G3">
-            <v>121.9</v>
-          </cell>
-          <cell r="H3">
-            <v>18.899999999999999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="F4">
-            <v>1.15E-2</v>
-          </cell>
-          <cell r="G4">
-            <v>-7.0000000000000001E-3</v>
-          </cell>
-          <cell r="H4">
-            <v>-1.2999999999999999E-3</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="F5">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="G5">
-            <v>1.1000000000000001E-3</v>
-          </cell>
-          <cell r="H5">
-            <v>3.85E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="6">
-          <cell r="C6">
-            <v>1.0699999999999999E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11">
-        <row r="4">
-          <cell r="H4">
-            <v>24</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12">
-        <row r="4">
-          <cell r="E4">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8478,39 +5748,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Class4"/>
-      <sheetName val="Options0"/>
-      <sheetName val="Options1"/>
       <sheetName val="Options2"/>
-      <sheetName val="Futures"/>
-      <sheetName val="Swaps"/>
-      <sheetName val="OptimalHedging"/>
-      <sheetName val="QuizBank4"/>
-      <sheetName val="O_Material"/>
-      <sheetName val="O_Discussion"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="6">
-          <cell r="C6">
-            <v>2.1837080457267475</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>-0.18370804572674748</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8832,79 +6073,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8BA7B8-F26D-3442-9338-39D695BA7AF8}">
   <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3">
       <c r="C3" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3">
       <c r="C4" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="C5" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3">
       <c r="C6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3">
       <c r="C7" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3">
       <c r="C8" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3">
       <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3">
       <c r="C11" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3">
       <c r="C12" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3">
       <c r="C13" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3">
       <c r="C14" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3">
       <c r="C15" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3">
       <c r="C16" s="1" t="s">
         <v>119</v>
       </c>
@@ -8924,19 +6165,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3">
       <c r="B4" s="1" t="s">
         <v>57</v>
       </c>
@@ -8944,7 +6185,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="B5" s="1" t="s">
         <v>59</v>
       </c>
@@ -8952,7 +6193,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3">
       <c r="B6" s="1" t="s">
         <v>60</v>
       </c>
@@ -8960,7 +6201,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3">
       <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
@@ -8968,7 +6209,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
@@ -8976,7 +6217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3">
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
@@ -8984,7 +6225,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3">
       <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
@@ -9006,32 +6247,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2">
       <c r="B5" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>163</v>
       </c>
@@ -9050,17 +6291,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2">
       <c r="B22" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2">
       <c r="B23" s="1" t="s">
         <v>172</v>
       </c>
@@ -9080,9 +6321,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9101,87 +6342,87 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="34.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2">
       <c r="B3" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2">
       <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2">
       <c r="B7" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2">
       <c r="B9" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2">
       <c r="B11" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2">
       <c r="B12" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2">
       <c r="B13" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2">
       <c r="B14" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2">
       <c r="B15" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2">
       <c r="B16" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
         <v>167</v>
       </c>
@@ -9204,17 +6445,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2">
       <c r="B22" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2">
       <c r="B23" s="1" t="s">
         <v>172</v>
       </c>
@@ -9234,34 +6475,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.33203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="4"/>
-    <col min="2" max="2" width="28.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.33203125" style="4"/>
+    <col min="1" max="1" width="2.375" style="4"/>
+    <col min="2" max="2" width="28.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.375" style="4"/>
     <col min="4" max="4" width="28.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="46.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.33203125" style="4"/>
-    <col min="10" max="10" width="40.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" style="4"/>
+    <col min="9" max="9" width="2.375" style="4"/>
+    <col min="10" max="10" width="40.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.375" style="4"/>
     <col min="12" max="12" width="37.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="2.33203125" style="4"/>
+    <col min="13" max="16384" width="2.375" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
@@ -9281,7 +6522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
@@ -9301,7 +6542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
@@ -9321,7 +6562,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
@@ -9335,7 +6576,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="F10" s="4" t="s">
         <v>34</v>
       </c>
@@ -9349,7 +6590,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12">
       <c r="F11" s="4" t="s">
         <v>38</v>
       </c>
@@ -9360,7 +6601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="H12" s="4" t="s">
         <v>41</v>
       </c>
@@ -9368,7 +6609,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="H13" s="4" t="s">
         <v>43</v>
       </c>
@@ -9376,7 +6617,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="H14" s="4" t="s">
         <v>45</v>
       </c>
@@ -9384,27 +6625,27 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="H15" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="H16" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8">
       <c r="H17" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:8">
       <c r="H18" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:8">
       <c r="H19" s="4" t="s">
         <v>50</v>
       </c>
@@ -9426,16 +6667,18 @@
   </sheetPr>
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="37.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3">
       <c r="B2" s="17" t="s">
         <v>120</v>
       </c>
@@ -9443,7 +6686,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
         <v>118</v>
       </c>
@@ -9451,7 +6694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3">
       <c r="B4" s="1" t="s">
         <v>116</v>
       </c>
@@ -9459,7 +6702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="B5" s="1" t="s">
         <v>117</v>
       </c>
@@ -9467,7 +6710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3">
       <c r="B6" s="1" t="s">
         <v>122</v>
       </c>
@@ -9475,7 +6718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3">
       <c r="B7" s="1" t="s">
         <v>123</v>
       </c>
@@ -9483,7 +6726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3">
       <c r="B8" s="1" t="s">
         <v>119</v>
       </c>
@@ -9491,22 +6734,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3">
       <c r="B10" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3">
       <c r="B11" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3">
       <c r="B12" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3">
       <c r="B13" s="1" t="s">
         <v>169</v>
       </c>
@@ -9527,9 +6770,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9546,19 +6789,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="27.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="27.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.875" style="1"/>
     <col min="7" max="7" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="8" max="9" width="10.875" style="1"/>
     <col min="10" max="10" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="11" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10">
       <c r="F2" s="18" t="s">
         <v>107</v>
       </c>
@@ -9573,7 +6816,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10">
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -9595,7 +6838,7 @@
         <v>0.98522167487684742</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10">
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
@@ -9617,7 +6860,7 @@
         <v>0.9706617486471405</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10">
       <c r="B5" s="1" t="s">
         <v>126</v>
       </c>
@@ -9639,7 +6882,7 @@
         <v>0.95631699374102519</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10">
       <c r="B6" s="1" t="s">
         <v>114</v>
       </c>
@@ -9661,7 +6904,7 @@
         <v>0.94218423028672449</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10">
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -9677,7 +6920,7 @@
         <v>0.92826032540563996</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10">
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -9693,7 +6936,7 @@
         <v>0.91454219251787205</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10">
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -9709,7 +6952,7 @@
         <v>0.90102679065800217</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10">
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -9725,7 +6968,7 @@
         <v>0.88771112380098749</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10">
       <c r="F11" s="1">
         <v>9</v>
       </c>
@@ -9741,7 +6984,7 @@
         <v>0.87459224019801729</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10">
       <c r="F12" s="1">
         <v>10</v>
       </c>
@@ -9757,7 +7000,7 @@
         <v>0.86166723172218462</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -9775,7 +7018,7 @@
         <v>0.8489332332238273</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -9789,7 +7032,7 @@
         <v>0.83638742189539661</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -9803,7 +7046,7 @@
         <v>0.82402701664571099</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -9817,7 +7060,7 @@
         <v>0.81184927748345925</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10">
       <c r="I17" s="1">
         <v>15</v>
       </c>
@@ -9826,7 +7069,7 @@
         <v>0.79985150490981216</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10">
       <c r="I18" s="1">
         <v>16</v>
       </c>
@@ -9835,7 +7078,7 @@
         <v>0.78803103932001206</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10">
       <c r="B19" s="22"/>
       <c r="I19" s="1">
         <v>17</v>
@@ -9845,7 +7088,7 @@
         <v>0.77638526041380518</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10">
       <c r="I20" s="1">
         <v>18</v>
       </c>
@@ -9854,7 +7097,7 @@
         <v>0.76491158661458636</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10">
       <c r="I21" s="1">
         <v>19</v>
       </c>
@@ -9863,7 +7106,7 @@
         <v>0.7536074744971295</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10">
       <c r="I22" s="1">
         <v>20</v>
       </c>
@@ -9872,7 +7115,7 @@
         <v>0.74247041822377313</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10">
       <c r="J23" s="23">
         <f>(SUM(J3:J22)*C5/2+J22)*C3</f>
         <v>2171686.3878508247</v>
@@ -9890,54 +7133,54 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.875" style="1"/>
     <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4">
       <c r="B5" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4">
       <c r="D7" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4">
       <c r="D8" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4">
       <c r="D9" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4">
       <c r="D10" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4">
       <c r="D11" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4">
       <c r="B13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4">
       <c r="D15" s="1" t="s">
         <v>83</v>
       </c>
@@ -9957,19 +7200,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="27.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="27.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.875" style="1"/>
     <col min="7" max="7" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="12" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10">
       <c r="F2" s="18" t="s">
         <v>107</v>
       </c>
@@ -9986,7 +7229,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10">
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -10013,7 +7256,7 @@
         <v>77669.902912621357</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10">
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
@@ -10040,7 +7283,7 @@
         <v>75407.672730700346</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10">
       <c r="B5" s="1" t="s">
         <v>126</v>
       </c>
@@ -10067,7 +7310,7 @@
         <v>73211.332748252767</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10">
       <c r="B6" s="1" t="s">
         <v>114</v>
       </c>
@@ -10094,7 +7337,7 @@
         <v>71078.963833255126</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10">
       <c r="F7" s="1">
         <v>5</v>
       </c>
@@ -10115,7 +7358,7 @@
         <v>69008.702750733122</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10">
       <c r="F8" s="1">
         <v>6</v>
       </c>
@@ -10136,7 +7379,7 @@
         <v>66998.740534692362</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10">
       <c r="F9" s="1">
         <v>7</v>
       </c>
@@ -10157,7 +7400,7 @@
         <v>65047.320907468304</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10">
       <c r="F10" s="1">
         <v>8</v>
       </c>
@@ -10178,7 +7421,7 @@
         <v>63152.738745114861</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10">
       <c r="B11" s="22"/>
       <c r="F11" s="1">
         <v>9</v>
@@ -10200,7 +7443,7 @@
         <v>61313.338587490158</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10">
       <c r="B12" s="24"/>
       <c r="F12" s="1">
         <v>10</v>
@@ -10222,7 +7465,7 @@
         <v>1547715.3429851884</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10">
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -10234,14 +7477,14 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -10254,7 +7497,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -10269,7 +7512,7 @@
         <v>18468997.692366112</v>
       </c>
     </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:11">
       <c r="I18" s="26" t="s">
         <v>132</v>
       </c>
@@ -10277,7 +7520,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="9:11">
       <c r="I19" s="12">
         <f>SUM(I3:I12)</f>
         <v>2170604.0567355165</v>
@@ -10287,7 +7530,7 @@
         <v>2170604.0567355165</v>
       </c>
     </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:11">
       <c r="I21" s="18" t="s">
         <v>134</v>
       </c>
@@ -10295,7 +7538,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:11">
       <c r="I22" s="13">
         <f>I16/I19</f>
         <v>8.5086903044595754</v>
@@ -10305,7 +7548,7 @@
         <v>8.5086903044595754</v>
       </c>
     </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:11">
       <c r="K23" s="23"/>
     </row>
   </sheetData>
@@ -10323,21 +7566,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1"/>
+    <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9">
       <c r="E2" s="11" t="s">
         <v>115</v>
       </c>
@@ -10354,7 +7597,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9">
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -10380,7 +7623,7 @@
         <v>79207.920792079211</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9">
       <c r="B4" s="1" t="s">
         <v>113</v>
       </c>
@@ -10406,7 +7649,7 @@
         <v>77652.939891771239</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" s="1" t="s">
         <v>114</v>
       </c>
@@ -10432,7 +7675,7 @@
         <v>75385.786763763565</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="E6" s="15">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10452,7 +7695,7 @@
         <v>72476.051583980399</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="E7" s="15">
         <v>0.03</v>
       </c>
@@ -10472,11 +7715,11 @@
         <v>1794226.2715190614</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9">
       <c r="G8" s="12"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9">
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -10485,15 +7728,15 @@
         <v>2098948.9705506559</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9">
       <c r="G10" s="12"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9">
       <c r="G11" s="12"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9">
       <c r="G12" s="12"/>
       <c r="I12" s="13"/>
     </row>
@@ -10512,21 +7755,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1"/>
+    <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9">
       <c r="E2" s="14" t="s">
         <v>115</v>
       </c>
@@ -10543,7 +7786,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9">
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -10569,7 +7812,7 @@
         <v>79207.920792079211</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9">
       <c r="B4" s="1" t="s">
         <v>113</v>
       </c>
@@ -10595,7 +7838,7 @@
         <v>78233.169179974808</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" s="1" t="s">
         <v>168</v>
       </c>
@@ -10621,7 +7864,7 @@
         <v>75385.786763763565</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="E6" s="15">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10641,7 +7884,7 @@
         <v>72476.051583980399</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="E7" s="15">
         <v>0.03</v>
       </c>
@@ -10661,11 +7904,11 @@
         <v>1691230.3435941758</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9">
       <c r="G8" s="12"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9">
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -10674,15 +7917,15 @@
         <v>1996533.2719139738</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9">
       <c r="G10" s="12"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9">
       <c r="G11" s="12"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9">
       <c r="G12" s="12"/>
       <c r="I12" s="13"/>
     </row>
@@ -10701,18 +7944,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="12.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="3" max="3" width="12.375" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19">
       <c r="C5" s="1"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19">
       <c r="B7" s="1">
         <v>1</v>
       </c>
@@ -10720,7 +7963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19">
       <c r="B8" s="1">
         <v>2</v>
       </c>
@@ -10733,7 +7976,7 @@
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19">
       <c r="B9" s="1">
         <v>3</v>
       </c>
@@ -10746,7 +7989,7 @@
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19">
       <c r="B10" s="1">
         <v>4</v>
       </c>
@@ -10759,7 +8002,7 @@
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19">
       <c r="B11" s="1">
         <v>5</v>
       </c>
@@ -10772,7 +8015,7 @@
       <c r="R11" s="21"/>
       <c r="S11" s="21"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19">
       <c r="B12" s="1">
         <v>6</v>
       </c>
@@ -10780,7 +8023,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19">
       <c r="B13" s="1">
         <v>7</v>
       </c>
@@ -10788,7 +8031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19">
       <c r="B14" s="1">
         <v>8</v>
       </c>
@@ -10796,7 +8039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19">
       <c r="B15" s="1">
         <v>9</v>
       </c>
@@ -10804,7 +8047,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19">
       <c r="B16" s="1">
         <v>10</v>
       </c>
@@ -10812,7 +8055,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3">
       <c r="B17" s="1">
         <v>11</v>
       </c>
@@ -10820,7 +8063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3">
       <c r="B18" s="1">
         <v>12</v>
       </c>
@@ -10828,7 +8071,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3">
       <c r="B19" s="1">
         <v>13</v>
       </c>
@@ -10836,7 +8079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3">
       <c r="B20" s="1">
         <v>14</v>
       </c>
@@ -10844,7 +8087,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3">
       <c r="B21" s="1">
         <v>15</v>
       </c>
@@ -10852,7 +8095,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3">
       <c r="B23" s="22"/>
     </row>
   </sheetData>
@@ -10872,12 +8115,12 @@
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6">
       <c r="B4" s="27">
         <v>1</v>
       </c>
@@ -10891,26 +8134,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6">
       <c r="F5" s="27">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6">
       <c r="F6" s="27">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6">
       <c r="F8" s="28">
         <f>B4*F4+C4*F5+D4*F6</f>
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2">
       <c r="B23" s="22"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2">
       <c r="B24" s="22"/>
     </row>
   </sheetData>
@@ -10929,12 +8172,12 @@
       <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8">
       <c r="B4" s="27">
         <v>1</v>
       </c>
@@ -10954,7 +8197,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8">
       <c r="F5" s="27">
         <v>4</v>
       </c>
@@ -10965,7 +8208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8">
       <c r="F6" s="27">
         <v>7</v>
       </c>
@@ -10976,7 +8219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8">
       <c r="F8" s="28">
         <f>B4*F4+C4*F5+D4*F6</f>
         <v>30</v>
@@ -10990,10 +8233,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2">
       <c r="B23" s="22"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2">
       <c r="B24" s="22"/>
     </row>
   </sheetData>
@@ -11010,12 +8253,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="2" t="s">
         <v>173</v>
       </c>
@@ -11040,67 +8283,67 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3">
       <c r="B2" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3">
       <c r="C4" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="C5" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3">
       <c r="C6" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3">
       <c r="B8" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3">
       <c r="C10" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3">
       <c r="C11" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3">
       <c r="C13" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3">
       <c r="C14" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3">
       <c r="C16" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3">
       <c r="C17" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3">
       <c r="C19" s="1" t="s">
         <v>170</v>
       </c>
@@ -11125,37 +8368,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2">
       <c r="B3" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2">
       <c r="B5" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2">
       <c r="B6" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2">
       <c r="B8" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2">
       <c r="B9" s="9" t="s">
         <v>94</v>
       </c>
@@ -11180,17 +8423,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3">
       <c r="B2" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3">
       <c r="B3" s="8" t="s">
         <v>145</v>
       </c>
@@ -11198,7 +8441,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3">
       <c r="B4" s="8" t="s">
         <v>146</v>
       </c>
@@ -11206,7 +8449,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3">
       <c r="B5" s="8" t="s">
         <v>147</v>
       </c>
@@ -11214,7 +8457,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3">
       <c r="B6" s="8" t="s">
         <v>148</v>
       </c>
@@ -11222,7 +8465,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3">
       <c r="B7" s="8" t="s">
         <v>149</v>
       </c>
@@ -11230,17 +8473,17 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2">
       <c r="B18" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2">
       <c r="B19" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2">
       <c r="B20" s="8" t="s">
         <v>144</v>
       </c>
@@ -11260,9 +8503,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11281,27 +8524,27 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="16384" width="10.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2">
       <c r="B3" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2">
       <c r="B5" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2">
       <c r="B6" s="9" t="s">
         <v>96</v>
       </c>
@@ -11325,42 +8568,42 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2">
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
@@ -11383,32 +8626,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2">
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>